<commit_message>
Added Colin's probabilities of transitions, and added the outbreaks
</commit_message>
<xml_diff>
--- a/DefaultValues.xlsx
+++ b/DefaultValues.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mes_documents\a_ABSys\DIGITAF\WP2farmers\task2.2_treecropperformance\BayesianPestModel\BayesianPestModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mes_documents\a_ABSys\DIGITAF\WP2farmers\task2.2_treecropperformance\ColinsPestModel\BooleanPestModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="8868" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="8868"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
     <sheet name="Effects" sheetId="2" r:id="rId2"/>
-    <sheet name="Transitions" sheetId="3" r:id="rId3"/>
+    <sheet name="Transitions" sheetId="6" r:id="rId3"/>
     <sheet name="initialisation" sheetId="4" r:id="rId4"/>
+    <sheet name="TransitionsRandom" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="46">
   <si>
     <t>Trees</t>
   </si>
@@ -150,6 +151,21 @@
   </si>
   <si>
     <t>initAt1</t>
+  </si>
+  <si>
+    <t>Pests_Yield_Diseases_Trees</t>
+  </si>
+  <si>
+    <t>Weeds_Pests_Trees</t>
+  </si>
+  <si>
+    <t>Diseases_Weeds_Pests</t>
+  </si>
+  <si>
+    <t>Diseases_NaturalEnemies_Trees_Weeds</t>
+  </si>
+  <si>
+    <t>Pests_Trees_Weeds_Diseases</t>
   </si>
 </sst>
 </file>
@@ -185,8 +201,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,12 +499,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -497,12 +514,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -694,10 +711,13 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.5546875" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -706,7 +726,7 @@
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D1" t="s">
@@ -718,1090 +738,1090 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D2">
-        <v>7.5722751673310995E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="E2">
-        <v>0.59551456011831805</v>
+        <v>1.375E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D3">
-        <v>6.3112640287727104E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>0.96565018338151298</v>
+        <v>6.2500000000000003E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
+        <v>41</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>0.52708933828398596</v>
+        <v>6.6250000000000003E-2</v>
       </c>
       <c r="E4">
-        <v>0.35393159370869398</v>
+        <v>3.7499999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>0.51679203868843604</v>
+        <v>3.6249999999999998E-2</v>
       </c>
       <c r="E5">
-        <v>0.41492157406173602</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>0.93634163937531401</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E6">
-        <v>0.274775707628578</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>0.58500494598411001</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E7">
-        <v>0.39382694079540698</v>
+        <v>6.2500000000000003E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>0.82258893270045497</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>0.37107031280174901</v>
+        <v>1.125E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>0.91760827088728503</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="E9">
-        <v>0.33750857645645699</v>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>0.426671832799911</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E10">
-        <v>0.14933656831271899</v>
+        <v>3.7499999999999999E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D11">
-        <v>0.77193008735775903</v>
+        <v>0.03</v>
       </c>
       <c r="E11">
-        <v>0.40413990197703198</v>
+        <v>2.1250000000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D12">
-        <v>0.74202324310317602</v>
+        <v>0.08</v>
       </c>
       <c r="E12">
-        <v>9.1849292162805796E-2</v>
+        <v>6.2500000000000003E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D13">
-        <v>0.136484595248476</v>
+        <v>1.6250000000000001E-2</v>
       </c>
       <c r="E13">
-        <v>0.78021971811540403</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
+        <v>41</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D14">
-        <v>0.72794769494794298</v>
+        <v>2.375E-2</v>
       </c>
       <c r="E14">
-        <v>0.83230292727239397</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D15">
-        <v>0.14980619167909001</v>
+        <v>3.7499999999999999E-3</v>
       </c>
       <c r="E15">
-        <v>0.216208771103993</v>
+        <v>3.3750000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
+        <v>41</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>0.44211234850809</v>
+        <v>0.03</v>
       </c>
       <c r="E16">
-        <v>0.67715571378357697</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D17">
-        <v>0.15343800745904401</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E17">
-        <v>0.34303304110653698</v>
+        <v>1.25E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D18">
-        <v>0.995425845962018</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="E18">
-        <v>0.54110573232173897</v>
+        <v>3.7499999999999999E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D19">
-        <v>0.16280007548630199</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="E19">
-        <v>0.37379710818640899</v>
+        <v>1.375E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D20">
-        <v>0.24537556408904501</v>
+        <v>3.3750000000000002E-2</v>
       </c>
       <c r="E20">
-        <v>0.98175280750729099</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
+        <v>42</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D21">
-        <v>0.26023560762405401</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E21">
-        <v>0.49823095952160701</v>
+        <v>1.125E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D22">
-        <v>0.69489655457437005</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="E22">
-        <v>0.82299119583331004</v>
+        <v>1.375E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
+        <v>42</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D23">
-        <v>0.12005190900526901</v>
+        <v>8.8749999999999996E-2</v>
       </c>
       <c r="E23">
-        <v>0.69059909577481404</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D24">
-        <v>0.106446550460532</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E24">
-        <v>0.80850512627512205</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D25">
-        <v>0.41917007905431097</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E25">
-        <v>0.37076899176463501</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" t="s">
-        <v>18</v>
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D26">
-        <v>0.79250224540010095</v>
+        <v>0.14374999999999999</v>
       </c>
       <c r="E26">
-        <v>0.69214625330641899</v>
+        <v>3.3750000000000002E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>17</v>
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D27">
-        <v>0.37991033121943502</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E27">
-        <v>0.76480988203547895</v>
+        <v>0.23125000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
+        <v>43</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="D28">
-        <v>0.62525192275643304</v>
+        <v>1.6250000000000001E-2</v>
       </c>
       <c r="E28">
-        <v>0.88142176740802802</v>
+        <v>0.21875</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D29">
-        <v>8.3479727618396304E-4</v>
+        <v>3.125E-2</v>
       </c>
       <c r="E29">
-        <v>0.24910907959565501</v>
+        <v>9.1249999999999998E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
+        <v>43</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="D30">
-        <v>0.26877350336872002</v>
+        <v>0.03</v>
       </c>
       <c r="E30">
-        <v>0.54509200225584198</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="D31">
-        <v>0.43335433350876001</v>
+        <v>2.75E-2</v>
       </c>
       <c r="E31">
-        <v>0.721770846750587</v>
+        <v>0.23125000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D32">
-        <v>0.51549431704916104</v>
+        <v>0.03</v>
       </c>
       <c r="E32">
-        <v>0.94930816860869505</v>
+        <v>0.18124999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
+        <v>43</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D33">
-        <v>0.47204085276462099</v>
+        <v>3.6249999999999998E-2</v>
       </c>
       <c r="E33">
-        <v>0.6440404439345</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D34">
-        <v>0.51032524462789297</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E34">
-        <v>5.1928530680015697E-2</v>
+        <v>2.6249999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>34</v>
+        <v>44</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D35">
-        <v>0.22947835549712201</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="E35">
-        <v>8.7465581484138993E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D36">
-        <v>0.53831722564064</v>
+        <v>0.1075</v>
       </c>
       <c r="E36">
-        <v>0.67046573432162404</v>
+        <v>8.7500000000000008E-3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" t="s">
-        <v>32</v>
+        <v>44</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>0.36570540140382901</v>
+        <v>0.1</v>
       </c>
       <c r="E37">
-        <v>0.37364647351205299</v>
+        <v>1.375E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D38">
-        <v>0.62112239236012101</v>
+        <v>6.8750000000000006E-2</v>
       </c>
       <c r="E38">
-        <v>0.207937398459762</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D39">
-        <v>0.94928468461148396</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E39">
-        <v>8.7214396800845903E-2</v>
+        <v>1.8749999999999999E-2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" t="s">
-        <v>29</v>
+        <v>44</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D40">
-        <v>0.56651913747191396</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="E40">
-        <v>0.56678240164183102</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D41">
-        <v>0.71041499730199598</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E41">
-        <v>4.3158981250598999E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D42">
-        <v>0.36864572833292197</v>
+        <v>4.8750000000000002E-2</v>
       </c>
       <c r="E42">
-        <v>0.47893853951245502</v>
+        <v>8.7499999999999994E-2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" t="s">
-        <v>34</v>
+        <v>44</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D43">
-        <v>0.69216222502291203</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E43">
-        <v>0.45592127298004897</v>
+        <v>9.7500000000000003E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D44">
-        <v>0.86562832724302996</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="E44">
-        <v>0.162284540245309</v>
+        <v>8.2500000000000004E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" t="s">
-        <v>32</v>
+        <v>44</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D45">
-        <v>0.53120138240046799</v>
+        <v>3.125E-2</v>
       </c>
       <c r="E45">
-        <v>8.8218968128785505E-2</v>
+        <v>8.2500000000000004E-2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D46">
-        <v>0.89231432671658695</v>
+        <v>3.6249999999999998E-2</v>
       </c>
       <c r="E46">
-        <v>0.34194001439027499</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" t="s">
-        <v>30</v>
+        <v>44</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D47">
-        <v>0.19866180256940399</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E47">
-        <v>5.2457021316513398E-2</v>
+        <v>3.3750000000000002E-2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C48" t="s">
-        <v>29</v>
+        <v>44</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D48">
-        <v>0.649239981779829</v>
+        <v>4.8750000000000002E-2</v>
       </c>
       <c r="E48">
-        <v>0.74915681104175702</v>
+        <v>8.7499999999999994E-2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>28</v>
-      </c>
-      <c r="C49" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D49">
-        <v>0.37903324328362897</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E49">
-        <v>0.87558189150877297</v>
+        <v>3.3750000000000002E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
-      </c>
-      <c r="C50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D50">
-        <v>0.100152868544683</v>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="E50">
-        <v>0.93015649495646402</v>
+        <v>0.3175</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="D51">
-        <v>0.78732494497671701</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E51">
-        <v>4.8116832273080903E-2</v>
+        <v>0.10249999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D52">
-        <v>0.831464249407873</v>
+        <v>0.04</v>
       </c>
       <c r="E52">
-        <v>0.54302761075086903</v>
+        <v>0.1225</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D53">
-        <v>0.509076704736799</v>
+        <v>0.11749999999999999</v>
       </c>
       <c r="E53">
-        <v>0.43560146237723502</v>
+        <v>5.6250000000000001E-2</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D54">
-        <v>0.70865745516493905</v>
+        <v>0.14249999999999999</v>
       </c>
       <c r="E54">
-        <v>0.55997679498978004</v>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" t="s">
-        <v>21</v>
+        <v>45</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D55">
-        <v>0.37805748172104398</v>
+        <v>0.1525</v>
       </c>
       <c r="E55">
-        <v>2.6489477837458301E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" t="s">
+        <v>45</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D56">
-        <v>0.52326072682626501</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="E56">
-        <v>0.10301005677320101</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D57">
-        <v>0.58827503980137397</v>
+        <v>0.13</v>
       </c>
       <c r="E57">
-        <v>0.67773858876898896</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" t="s">
-        <v>18</v>
+        <v>45</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D58">
-        <v>0.98270523478277005</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="E58">
-        <v>0.214156469097361</v>
+        <v>3.2500000000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" t="s">
-        <v>17</v>
+        <v>45</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D59">
-        <v>0.39380306610837601</v>
+        <v>0.1275</v>
       </c>
       <c r="E59">
-        <v>0.96951443888247002</v>
+        <v>6.7500000000000004E-2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" t="s">
-        <v>16</v>
+        <v>45</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D60">
-        <v>0.59393981983885202</v>
+        <v>0.20250000000000001</v>
       </c>
       <c r="E60">
-        <v>0.25312645966187097</v>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D61">
-        <v>0.70167690003290795</v>
+        <v>0.02</v>
       </c>
       <c r="E61">
-        <v>0.35141206253320001</v>
+        <v>0.21124999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" t="s">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D62">
-        <v>0.83505725301802203</v>
+        <v>3.2500000000000001E-2</v>
       </c>
       <c r="E62">
-        <v>0.88823185744695399</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" t="s">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D63">
-        <v>0.411600720603019</v>
+        <v>0.13</v>
       </c>
       <c r="E63">
-        <v>0.91363238776102695</v>
+        <v>2.6249999999999999E-2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>11</v>
-      </c>
-      <c r="C64" t="s">
-        <v>12</v>
+        <v>45</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D64">
-        <v>0.87770282616838802</v>
+        <v>0.155</v>
       </c>
       <c r="E64">
-        <v>0.554062416311353</v>
+        <v>4.3749999999999997E-2</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" t="s">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D65">
-        <v>7.5033113360404996E-2</v>
+        <v>4.6249999999999999E-2</v>
       </c>
       <c r="E65">
-        <v>0.80062004108913198</v>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1832,4 +1852,1124 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>7.5722751673310995E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.59551456011831805</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>6.3112640287727104E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.96565018338151298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4">
+        <v>0.52708933828398596</v>
+      </c>
+      <c r="E4">
+        <v>0.35393159370869398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5">
+        <v>0.51679203868843604</v>
+      </c>
+      <c r="E5">
+        <v>0.41492157406173602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>0.93634163937531401</v>
+      </c>
+      <c r="E6">
+        <v>0.274775707628578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>0.58500494598411001</v>
+      </c>
+      <c r="E7">
+        <v>0.39382694079540698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>0.82258893270045497</v>
+      </c>
+      <c r="E8">
+        <v>0.37107031280174901</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>0.91760827088728503</v>
+      </c>
+      <c r="E9">
+        <v>0.33750857645645699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>0.426671832799911</v>
+      </c>
+      <c r="E10">
+        <v>0.14933656831271899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>0.77193008735775903</v>
+      </c>
+      <c r="E11">
+        <v>0.40413990197703198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>0.74202324310317602</v>
+      </c>
+      <c r="E12">
+        <v>9.1849292162805796E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0.136484595248476</v>
+      </c>
+      <c r="E13">
+        <v>0.78021971811540403</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>0.72794769494794298</v>
+      </c>
+      <c r="E14">
+        <v>0.83230292727239397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>0.14980619167909001</v>
+      </c>
+      <c r="E15">
+        <v>0.216208771103993</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>0.44211234850809</v>
+      </c>
+      <c r="E16">
+        <v>0.67715571378357697</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>0.15343800745904401</v>
+      </c>
+      <c r="E17">
+        <v>0.34303304110653698</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>0.995425845962018</v>
+      </c>
+      <c r="E18">
+        <v>0.54110573232173897</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>0.16280007548630199</v>
+      </c>
+      <c r="E19">
+        <v>0.37379710818640899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>0.24537556408904501</v>
+      </c>
+      <c r="E20">
+        <v>0.98175280750729099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
+        <v>0.26023560762405401</v>
+      </c>
+      <c r="E21">
+        <v>0.49823095952160701</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>0.69489655457437005</v>
+      </c>
+      <c r="E22">
+        <v>0.82299119583331004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>0.12005190900526901</v>
+      </c>
+      <c r="E23">
+        <v>0.69059909577481404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>0.106446550460532</v>
+      </c>
+      <c r="E24">
+        <v>0.80850512627512205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25">
+        <v>0.41917007905431097</v>
+      </c>
+      <c r="E25">
+        <v>0.37076899176463501</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26">
+        <v>0.79250224540010095</v>
+      </c>
+      <c r="E26">
+        <v>0.69214625330641899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>0.37991033121943502</v>
+      </c>
+      <c r="E27">
+        <v>0.76480988203547895</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>0.62525192275643304</v>
+      </c>
+      <c r="E28">
+        <v>0.88142176740802802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>8.3479727618396304E-4</v>
+      </c>
+      <c r="E29">
+        <v>0.24910907959565501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>0.26877350336872002</v>
+      </c>
+      <c r="E30">
+        <v>0.54509200225584198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>0.43335433350876001</v>
+      </c>
+      <c r="E31">
+        <v>0.721770846750587</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32">
+        <v>0.51549431704916104</v>
+      </c>
+      <c r="E32">
+        <v>0.94930816860869505</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>0.47204085276462099</v>
+      </c>
+      <c r="E33">
+        <v>0.6440404439345</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34">
+        <v>0.51032524462789297</v>
+      </c>
+      <c r="E34">
+        <v>5.1928530680015697E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>0.22947835549712201</v>
+      </c>
+      <c r="E35">
+        <v>8.7465581484138993E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36">
+        <v>0.53831722564064</v>
+      </c>
+      <c r="E36">
+        <v>0.67046573432162404</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>0.36570540140382901</v>
+      </c>
+      <c r="E37">
+        <v>0.37364647351205299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <v>0.62112239236012101</v>
+      </c>
+      <c r="E38">
+        <v>0.207937398459762</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>0.94928468461148396</v>
+      </c>
+      <c r="E39">
+        <v>8.7214396800845903E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>0.56651913747191396</v>
+      </c>
+      <c r="E40">
+        <v>0.56678240164183102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41">
+        <v>0.71041499730199598</v>
+      </c>
+      <c r="E41">
+        <v>4.3158981250598999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>28</v>
+      </c>
+      <c r="C42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42">
+        <v>0.36864572833292197</v>
+      </c>
+      <c r="E42">
+        <v>0.47893853951245502</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43">
+        <v>0.69216222502291203</v>
+      </c>
+      <c r="E43">
+        <v>0.45592127298004897</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44">
+        <v>0.86562832724302996</v>
+      </c>
+      <c r="E44">
+        <v>0.162284540245309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45">
+        <v>0.53120138240046799</v>
+      </c>
+      <c r="E45">
+        <v>8.8218968128785505E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46">
+        <v>0.89231432671658695</v>
+      </c>
+      <c r="E46">
+        <v>0.34194001439027499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47">
+        <v>0.19866180256940399</v>
+      </c>
+      <c r="E47">
+        <v>5.2457021316513398E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48">
+        <v>0.649239981779829</v>
+      </c>
+      <c r="E48">
+        <v>0.74915681104175702</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49">
+        <v>0.37903324328362897</v>
+      </c>
+      <c r="E49">
+        <v>0.87558189150877297</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50">
+        <v>0.100152868544683</v>
+      </c>
+      <c r="E50">
+        <v>0.93015649495646402</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51">
+        <v>0.78732494497671701</v>
+      </c>
+      <c r="E51">
+        <v>4.8116832273080903E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52">
+        <v>0.831464249407873</v>
+      </c>
+      <c r="E52">
+        <v>0.54302761075086903</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53">
+        <v>0.509076704736799</v>
+      </c>
+      <c r="E53">
+        <v>0.43560146237723502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54">
+        <v>0.70865745516493905</v>
+      </c>
+      <c r="E54">
+        <v>0.55997679498978004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55">
+        <v>0.37805748172104398</v>
+      </c>
+      <c r="E55">
+        <v>2.6489477837458301E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56">
+        <v>0.52326072682626501</v>
+      </c>
+      <c r="E56">
+        <v>0.10301005677320101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57">
+        <v>0.58827503980137397</v>
+      </c>
+      <c r="E57">
+        <v>0.67773858876898896</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58">
+        <v>0.98270523478277005</v>
+      </c>
+      <c r="E58">
+        <v>0.214156469097361</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59">
+        <v>0.39380306610837601</v>
+      </c>
+      <c r="E59">
+        <v>0.96951443888247002</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>0.59393981983885202</v>
+      </c>
+      <c r="E60">
+        <v>0.25312645966187097</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>0.70167690003290795</v>
+      </c>
+      <c r="E61">
+        <v>0.35141206253320001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62">
+        <v>0.83505725301802203</v>
+      </c>
+      <c r="E62">
+        <v>0.88823185744695399</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63">
+        <v>0.411600720603019</v>
+      </c>
+      <c r="E63">
+        <v>0.91363238776102695</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>0.87770282616838802</v>
+      </c>
+      <c r="E64">
+        <v>0.554062416311353</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>7.5033113360404996E-2</v>
+      </c>
+      <c r="E65">
+        <v>0.80062004108913198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>